<commit_message>
[PeerSimple.js] 用 fon.base/Network.js 的 isPrivateIp() 来检测本地IP。 [server.js] 改进 node server -h 时的输出信息。
</commit_message>
<xml_diff>
--- a/doc/api.xlsx
+++ b/doc/api.xlsx
@@ -13,8 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="api" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="tic.crypto" sheetId="2" r:id="rId3"/>
+    <sheet name="tic.crypto" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="135">
   <si>
     <t>Block/</t>
   </si>
@@ -439,144 +438,6 @@
   </si>
   <si>
     <t>Peer/</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>主人</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>node.server</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>时光链</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>node.console</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>控制台</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>节点服务器</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>wallet</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>钱包</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>cloud</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>武玉娇</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>李超</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>徐稼生</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>链工坊</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>金丽</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>面向群体</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2C：个人用户</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2D：应用开发者</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2P：节点运营者</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2B：商业客户</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>*.market</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>市场</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>链云台</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>远景目标</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>应用链生态圈</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>浏览器</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>节点</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>链宝盒</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>产品</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>去中心的人人云平台</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>通用名</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>品牌名
-（方案2）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>品牌名
-（方案1）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>区块链云平台 BaaS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>每个人的私人银行+交易所</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -584,7 +445,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,30 +475,6 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -696,7 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -715,157 +552,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -876,21 +568,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:G6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
-  <tableColumns count="7">
-    <tableColumn id="1" name="产品" dataDxfId="7"/>
-    <tableColumn id="2" name="主人" dataDxfId="6"/>
-    <tableColumn id="3" name="通用名" dataDxfId="5"/>
-    <tableColumn id="4" name="品牌名_x000a_（方案1）" dataDxfId="4"/>
-    <tableColumn id="6" name="品牌名_x000a_（方案2）" dataDxfId="3"/>
-    <tableColumn id="5" name="面向群体" dataDxfId="2"/>
-    <tableColumn id="7" name="远景目标" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1620,161 +1297,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="18.796875" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" customWidth="1"/>
-    <col min="3" max="3" width="21.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.73046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="49.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="51.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="50.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="40.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>